<commit_message>
ticker.history piriod changed to 3d, keyword for record skipping changed from 'PLN' to 'none'
</commit_message>
<xml_diff>
--- a/portfel.xlsx
+++ b/portfel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="60" windowWidth="11292" windowHeight="5580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="60" windowWidth="11292" windowHeight="5580" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="portfel" sheetId="1" state="visible" r:id="rId1"/>
@@ -467,7 +467,7 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1013,7 +1013,7 @@
         <v>0.001</v>
       </c>
       <c r="D5" t="n">
-        <v>108007.7890625</v>
+        <v>108106.3671875</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>none</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1053,7 +1053,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>none</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">

</xml_diff>